<commit_message>
Adding excel spreadsheet to list of tracked files.
</commit_message>
<xml_diff>
--- a/Cophy package development.xlsx
+++ b/Cophy package development.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="26820" windowHeight="26360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="51440" yWindow="1440" windowWidth="27880" windowHeight="25560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ToDos" sheetId="1" r:id="rId1"/>
     <sheet name="Functions" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Functions!$B$2:$F$40</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
   <si>
     <t>ToDos for package cophy:</t>
   </si>
@@ -139,24 +142,9 @@
     <t>parsimulate.2PonH.infectionResponse</t>
   </si>
   <si>
-    <t>randomcophy</t>
-  </si>
-  <si>
     <t>simulate</t>
   </si>
   <si>
-    <t>simulate_cophys_HP</t>
-  </si>
-  <si>
-    <t>simulate_cophys_H</t>
-  </si>
-  <si>
-    <t>simulate_cophys_PonH</t>
-  </si>
-  <si>
-    <t>simulate_cophys_2PonH</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -205,24 +193,9 @@
     <t>convert</t>
   </si>
   <si>
-    <t>convert_HbranchesToPhylo</t>
-  </si>
-  <si>
-    <t>convert_PbranchesToPhylo</t>
-  </si>
-  <si>
-    <t>convert_2PbranchesToPhylo</t>
-  </si>
-  <si>
-    <t>convert_HPbranchesToCophylo</t>
-  </si>
-  <si>
     <t>convert_cophyloToBranches</t>
   </si>
   <si>
-    <t>convert_2PcophyloToBranches</t>
-  </si>
-  <si>
     <t>plot.cophy</t>
   </si>
   <si>
@@ -286,9 +259,6 @@
     <t>get_PHDistCorr</t>
   </si>
   <si>
-    <t>get</t>
-  </si>
-  <si>
     <t>plot</t>
   </si>
   <si>
@@ -340,13 +310,52 @@
     <t>rcophylo_PonH_Htrait</t>
   </si>
   <si>
-    <t>simulate_PonH_Htrait</t>
-  </si>
-  <si>
     <t>rcophy_PonH_HPtrait</t>
   </si>
   <si>
-    <t>simulate_PonH_HPtrait</t>
+    <t>rcophylo</t>
+  </si>
+  <si>
+    <t>- change rcophylo_PQonH so that it allows for different times of invasion?</t>
+  </si>
+  <si>
+    <t>- consolidate functions with host and parasite traits</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_HP</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_H</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_PonH</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_2PonH</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_PonH_HPtrait</t>
+  </si>
+  <si>
+    <t>simulate_cophylos_PonH_Htrait</t>
+  </si>
+  <si>
+    <t>- enable H.tree to have phylo format in the different rcophylo functions</t>
+  </si>
+  <si>
+    <t>convert_HPBranchesToCophylo</t>
+  </si>
+  <si>
+    <t>convert_HBranchesToPhylo</t>
+  </si>
+  <si>
+    <t>convert_PBranchesToPhylo</t>
+  </si>
+  <si>
+    <t>convert_PQCophyloToBranches</t>
+  </si>
+  <si>
+    <t>convert_PQBranchesToPhylo</t>
   </si>
 </sst>
 </file>
@@ -403,8 +412,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -431,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -442,6 +453,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +464,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -727,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B20"/>
+  <dimension ref="B2:B23"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -826,6 +839,21 @@
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -840,19 +868,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -873,74 +902,74 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" hidden="1">
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" hidden="1">
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" hidden="1">
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" hidden="1">
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" hidden="1">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -948,13 +977,13 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -962,13 +991,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -976,13 +1005,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -990,13 +1019,13 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -1004,16 +1033,16 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:6">
@@ -1021,30 +1050,30 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" hidden="1">
       <c r="B14" t="s">
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -1052,30 +1081,30 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" hidden="1">
       <c r="B16" t="s">
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -1083,356 +1112,363 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" hidden="1">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" hidden="1">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" hidden="1">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>107</v>
       </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" hidden="1">
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" hidden="1">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" hidden="1">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" hidden="1">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" hidden="1">
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" hidden="1">
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" hidden="1">
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" hidden="1">
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" hidden="1">
+      <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1">
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" hidden="1">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" t="s">
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" hidden="1">
+      <c r="B32" t="s">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" hidden="1">
+      <c r="B33" t="s">
         <v>67</v>
       </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" hidden="1">
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" hidden="1">
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" hidden="1">
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" hidden="1">
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" hidden="1">
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" hidden="1">
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" hidden="1">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="C40" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" t="s">
         <v>83</v>
       </c>
-      <c r="D31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" t="s">
-        <v>94</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:F40">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="simulate"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>